<commit_message>
ancho de banda y frecuencia
</commit_message>
<xml_diff>
--- a/docs/ccna_02.xlsx
+++ b/docs/ccna_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16C553E-F271-4645-BD3C-8149EDF0697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD377B3-0874-4566-BCB0-8BF2A6725527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5DA699B9-F984-43A8-847D-39D4CCE89DF4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
   <si>
     <t>bit</t>
   </si>
@@ -205,16 +205,81 @@
   </si>
   <si>
     <t>0/1</t>
+  </si>
+  <si>
+    <t>ANCHO DE BANDA</t>
+  </si>
+  <si>
+    <t>Kilobits/s</t>
+  </si>
+  <si>
+    <t>Bit/s</t>
+  </si>
+  <si>
+    <t>Megabits/s</t>
+  </si>
+  <si>
+    <t>Gigabit/s</t>
+  </si>
+  <si>
+    <t>Terabits/s</t>
+  </si>
+  <si>
+    <t>1000bps</t>
+  </si>
+  <si>
+    <t>1000Kbps</t>
+  </si>
+  <si>
+    <t>1000Mbps</t>
+  </si>
+  <si>
+    <t>1000Gbps</t>
+  </si>
+  <si>
+    <t>FRECUENCIA</t>
+  </si>
+  <si>
+    <t>Hertz</t>
+  </si>
+  <si>
+    <t>1 Ciclo/Segundo</t>
+  </si>
+  <si>
+    <t>KiloHertz</t>
+  </si>
+  <si>
+    <t>1000Hz</t>
+  </si>
+  <si>
+    <t>MegaHertz</t>
+  </si>
+  <si>
+    <t>1000KHz</t>
+  </si>
+  <si>
+    <t>GigaHertz</t>
+  </si>
+  <si>
+    <t>1000MHz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,15 +291,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -242,11 +319,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,19 +342,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -286,9 +391,33 @@
   <autoFilter ref="A4:D16" xr:uid="{6FF6FFF7-2D81-4952-9C43-6FE2632CBCB3}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{0D46ACDE-2FA3-4E37-BDD1-DBC60F6C2A4B}" name="Unidad" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B42C37AA-EF60-4104-B816-72AFF31918C8}" name="Equivalencia" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{5D3B9A44-5399-4256-A2DF-AFC1704164DE}" name="Potencia" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{B42C37AA-EF60-4104-B816-72AFF31918C8}" name="Equivalencia" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5D3B9A44-5399-4256-A2DF-AFC1704164DE}" name="Potencia" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{76E7A52E-95B2-4250-BBAB-6149E8B4E6D4}" name="Binario"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BACBDDF4-DD9E-4A3C-AC95-95CF0E71D8B7}" name="Tabla2" displayName="Tabla2" ref="F4:H9" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="F4:H9" xr:uid="{BACBDDF4-DD9E-4A3C-AC95-95CF0E71D8B7}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{C4D8DFB3-778D-4927-B614-B4FA819D7FAE}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{82A04101-A7B7-4CFA-9B48-6060B7B7F0D1}" name="Equivalencia" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CA9806D8-81EA-46CE-931F-A7D6DB4E2871}" name="Potencia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{C54F78C6-0ED2-48AC-952D-F39654D5D205}" name="Tabla3" displayName="Tabla3" ref="F12:H16" totalsRowShown="0">
+  <autoFilter ref="F12:H16" xr:uid="{C54F78C6-0ED2-48AC-952D-F39654D5D205}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{AE07FB80-353A-4ADA-AD18-DD7D97E33D66}" name="Unidad"/>
+    <tableColumn id="2" xr3:uid="{5FD31455-2541-4B68-B65D-B6CFBB83EA82}" name="Equivalencia"/>
+    <tableColumn id="3" xr3:uid="{77C8465B-3293-455C-9DA8-4999633770FC}" name="Potencia"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -591,21 +720,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDA46B8-4A74-4D58-8C25-62CE9C939A7B}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -619,12 +752,20 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="F3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -637,9 +778,18 @@
       <c r="D4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -651,9 +801,18 @@
       <c r="D5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -665,9 +824,18 @@
       <c r="D6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="F6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -679,9 +847,18 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -693,9 +870,18 @@
       <c r="D8" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="F8" t="s">
+        <v>61</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -707,9 +893,18 @@
       <c r="D9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="F9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -722,8 +917,8 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -735,9 +930,14 @@
       <c r="D11" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="F11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -749,9 +949,18 @@
       <c r="D12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="F12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -763,9 +972,18 @@
       <c r="D13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -777,9 +995,18 @@
       <c r="D14" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -791,9 +1018,18 @@
       <c r="D15" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -805,12 +1041,28 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <mergeCells count="3">
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F11:H11"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
tramas y tipos de dispositivos
</commit_message>
<xml_diff>
--- a/docs/ccna_02.xlsx
+++ b/docs/ccna_02.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EducacionIT\Documents\networks\CISCO\saves\ccna2-s10\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD377B3-0874-4566-BCB0-8BF2A6725527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F612F510-A89B-4318-93FD-257E70DBA675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5DA699B9-F984-43A8-847D-39D4CCE89DF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5DA699B9-F984-43A8-847D-39D4CCE89DF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Unidades" sheetId="1" r:id="rId1"/>
+    <sheet name="Enlace" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>bit</t>
   </si>
@@ -262,6 +263,126 @@
   </si>
   <si>
     <t>1000MHz</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>MDIX</t>
+  </si>
+  <si>
+    <t>Comandos</t>
+  </si>
+  <si>
+    <t>Parametros</t>
+  </si>
+  <si>
+    <t>Deteccion de interfaz cruzada (AUTO)</t>
+  </si>
+  <si>
+    <t>DUPLEX</t>
+  </si>
+  <si>
+    <t>envio y recepcion (HALF/FULL/AUTO)</t>
+  </si>
+  <si>
+    <t>SPEED</t>
+  </si>
+  <si>
+    <t>Ancho de banda (10/100/1000/AUTO)</t>
+  </si>
+  <si>
+    <t>CDP</t>
+  </si>
+  <si>
+    <t>Descubrimiento Vecino Cisco (ENABLE)</t>
+  </si>
+  <si>
+    <t>LLDP</t>
+  </si>
+  <si>
+    <t>Descubrimiento (TRANSMIT/RECEIVE)</t>
+  </si>
+  <si>
+    <t>Switches</t>
+  </si>
+  <si>
+    <t>FIJA</t>
+  </si>
+  <si>
+    <t>EXPANDIBLE</t>
+  </si>
+  <si>
+    <t>APILABLE</t>
+  </si>
+  <si>
+    <t>Poseen buses de expansion que permiten agregar nuevas interfaces.</t>
+  </si>
+  <si>
+    <t>Permiten la conexión entre varios, para funcionar como uno de mayor capacidad.</t>
+  </si>
+  <si>
+    <t>Metodo</t>
+  </si>
+  <si>
+    <t>Funcionamiento</t>
+  </si>
+  <si>
+    <t>Reenvian la trama apenas la reciben, sin verificar la misma.</t>
+  </si>
+  <si>
+    <t>Almacenan la trama en un buffer y la reenvia despues de verificarla</t>
+  </si>
+  <si>
+    <t>Leen los primeros 64B y luego realiza el envio de la misma.</t>
+  </si>
+  <si>
+    <t>Detalles</t>
+  </si>
+  <si>
+    <t>Tramas menores a 64B, productos de una colision</t>
+  </si>
+  <si>
+    <t>Tramas mayores a 1,5KB, por fallos en la interfaz</t>
+  </si>
+  <si>
+    <t>Throttle</t>
+  </si>
+  <si>
+    <t>Giant</t>
+  </si>
+  <si>
+    <t>Runt</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>Tramas descartadas, por desbordamiento de buffer</t>
+  </si>
+  <si>
+    <t>Tramas Corruptas, consecuencia de EMI o RFI</t>
+  </si>
+  <si>
+    <t>Jumbo</t>
+  </si>
+  <si>
+    <t>Tipos de Tramas</t>
+  </si>
+  <si>
+    <t>Tramas de 9KB, establecidas por configuracion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fragment-Free</t>
+  </si>
+  <si>
+    <t>Cut-Through</t>
+  </si>
+  <si>
+    <t>Store-N-Forward</t>
+  </si>
+  <si>
+    <t>Cantidad de interfaces predeterminada, sin capacidad de expansion</t>
   </si>
 </sst>
 </file>
@@ -334,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -353,11 +474,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -390,9 +526,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6FF6FFF7-2D81-4952-9C43-6FE2632CBCB3}" name="Tabla1" displayName="Tabla1" ref="A4:D16" totalsRowShown="0">
   <autoFilter ref="A4:D16" xr:uid="{6FF6FFF7-2D81-4952-9C43-6FE2632CBCB3}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0D46ACDE-2FA3-4E37-BDD1-DBC60F6C2A4B}" name="Unidad" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B42C37AA-EF60-4104-B816-72AFF31918C8}" name="Equivalencia" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{5D3B9A44-5399-4256-A2DF-AFC1704164DE}" name="Potencia" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{0D46ACDE-2FA3-4E37-BDD1-DBC60F6C2A4B}" name="Unidad" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B42C37AA-EF60-4104-B816-72AFF31918C8}" name="Equivalencia" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5D3B9A44-5399-4256-A2DF-AFC1704164DE}" name="Potencia" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{76E7A52E-95B2-4250-BBAB-6149E8B4E6D4}" name="Binario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -400,11 +536,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BACBDDF4-DD9E-4A3C-AC95-95CF0E71D8B7}" name="Tabla2" displayName="Tabla2" ref="F4:H9" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BACBDDF4-DD9E-4A3C-AC95-95CF0E71D8B7}" name="Tabla2" displayName="Tabla2" ref="F4:H9" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="F4:H9" xr:uid="{BACBDDF4-DD9E-4A3C-AC95-95CF0E71D8B7}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{C4D8DFB3-778D-4927-B614-B4FA819D7FAE}" name="Unidad"/>
-    <tableColumn id="2" xr3:uid="{82A04101-A7B7-4CFA-9B48-6060B7B7F0D1}" name="Equivalencia" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{82A04101-A7B7-4CFA-9B48-6060B7B7F0D1}" name="Equivalencia" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{CA9806D8-81EA-46CE-931F-A7D6DB4E2871}" name="Potencia"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -418,6 +554,50 @@
     <tableColumn id="1" xr3:uid="{AE07FB80-353A-4ADA-AD18-DD7D97E33D66}" name="Unidad"/>
     <tableColumn id="2" xr3:uid="{5FD31455-2541-4B68-B65D-B6CFBB83EA82}" name="Equivalencia"/>
     <tableColumn id="3" xr3:uid="{77C8465B-3293-455C-9DA8-4999633770FC}" name="Potencia"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4E22E949-A98A-4EBC-8023-6D2A69897782}" name="Tabla5" displayName="Tabla5" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{4E22E949-A98A-4EBC-8023-6D2A69897782}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9741EB9D-8A25-46E2-B75C-464551B14D5C}" name="Comandos"/>
+    <tableColumn id="2" xr3:uid="{10499CA0-686A-48D2-A684-E825287274B3}" name="Parametros"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{56FFE86F-806B-4FB6-A2AC-1FF90204B23D}" name="Tabla6" displayName="Tabla6" ref="A8:B11" totalsRowShown="0">
+  <autoFilter ref="A8:B11" xr:uid="{56FFE86F-806B-4FB6-A2AC-1FF90204B23D}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CF46A668-35DD-4E7A-B0AA-5A402841F3B1}" name="Switches" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{26741A7F-96B0-41C4-AC2A-FB6443F7C5C7}" name="Descripcion" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1C1541D3-FDC3-45E6-BA3E-829AA03D5AFF}" name="Tabla7" displayName="Tabla7" ref="D1:E6" totalsRowShown="0">
+  <autoFilter ref="D1:E6" xr:uid="{1C1541D3-FDC3-45E6-BA3E-829AA03D5AFF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5E642B6E-CBE6-4174-A922-638251C66A59}" name="Tipos de Tramas"/>
+    <tableColumn id="2" xr3:uid="{2FC8B58A-1F8F-4F12-83D1-20DE3083E6F1}" name="Detalles"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A5764858-988F-4F8B-9531-EB9B44615F84}" name="Tabla8" displayName="Tabla8" ref="D8:E11" totalsRowShown="0">
+  <autoFilter ref="D8:E11" xr:uid="{A5764858-988F-4F8B-9531-EB9B44615F84}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{03306FF0-1C74-4931-BA11-1AB874FA8516}" name="Metodo"/>
+    <tableColumn id="2" xr3:uid="{960C1F1B-06E7-4F17-914F-2C0BA893D8C6}" name="Funcionamiento"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -722,7 +902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDA46B8-4A74-4D58-8C25-62CE9C939A7B}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1065,4 +1245,172 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A25B4058-481C-4CED-8D46-38E88A84D9F1}">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>